<commit_message>
add rfuse results files
</commit_message>
<xml_diff>
--- a/rfuse/ext4_summary.xlsx
+++ b/rfuse/ext4_summary.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="busy" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="idle" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summary" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:AM11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +437,31 @@
           <t>lat_avg(ns)</t>
         </is>
       </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>BW(MiB/s)</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>IOPS</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>lat_avg(ns)</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>lat_p95(ns)</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>lat_p99(ns)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="C2" t="n">
@@ -476,6 +500,60 @@
       <c r="N2" t="n">
         <v>4</v>
       </c>
+      <c r="V2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" t="n">
+        <v>2</v>
+      </c>
+      <c r="X2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -488,6 +566,16 @@
           <t>bs</t>
         </is>
       </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>workload</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>bs</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -536,6 +624,70 @@
       <c r="N4" t="n">
         <v>386.48</v>
       </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>randread</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>128k</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>380</v>
+      </c>
+      <c r="W4" t="n">
+        <v>705</v>
+      </c>
+      <c r="X4" t="n">
+        <v>1011</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1249</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>3038</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>5641</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>8084</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>9990</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>328.52</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>352.26</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>364.82</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>381.4</v>
+      </c>
+      <c r="AH4" t="n">
+        <v/>
+      </c>
+      <c r="AI4" t="n">
+        <v/>
+      </c>
+      <c r="AJ4" t="n">
+        <v/>
+      </c>
+      <c r="AK4" t="n">
+        <v/>
+      </c>
+      <c r="AL4" t="n">
+        <v/>
+      </c>
+      <c r="AM4" t="n">
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
@@ -579,6 +731,65 @@
       <c r="N5" t="n">
         <v>21505.17</v>
       </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>4k</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v/>
+      </c>
+      <c r="W5" t="n">
+        <v/>
+      </c>
+      <c r="X5" t="n">
+        <v/>
+      </c>
+      <c r="Y5" t="n">
+        <v/>
+      </c>
+      <c r="Z5" t="n">
+        <v>5818</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>11</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>5720.45</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>10969.64</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>15906</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>21039.03</v>
+      </c>
+      <c r="AH5" t="n">
+        <v/>
+      </c>
+      <c r="AI5" t="n">
+        <v/>
+      </c>
+      <c r="AJ5" t="n">
+        <v/>
+      </c>
+      <c r="AK5" t="n">
+        <v/>
+      </c>
+      <c r="AL5" t="n">
+        <v/>
+      </c>
+      <c r="AM5" t="n">
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -627,6 +838,70 @@
       <c r="N6" t="n">
         <v>57.42</v>
       </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>randwrite</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>128k</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>186</v>
+      </c>
+      <c r="W6" t="n">
+        <v>197</v>
+      </c>
+      <c r="X6" t="n">
+        <v>249</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>290</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>1484</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1572</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>1989</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>2323</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>61.78</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>59.39</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>61.27</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>69.94</v>
+      </c>
+      <c r="AH6" t="n">
+        <v/>
+      </c>
+      <c r="AI6" t="n">
+        <v/>
+      </c>
+      <c r="AJ6" t="n">
+        <v/>
+      </c>
+      <c r="AK6" t="n">
+        <v/>
+      </c>
+      <c r="AL6" t="n">
+        <v/>
+      </c>
+      <c r="AM6" t="n">
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
@@ -670,6 +945,65 @@
       <c r="N7" t="n">
         <v>2477.47</v>
       </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>4k</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v/>
+      </c>
+      <c r="W7" t="n">
+        <v>140</v>
+      </c>
+      <c r="X7" t="n">
+        <v>150</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>185</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>35</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>38</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>47</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>30723</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>60528</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>82994</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>107703</v>
+      </c>
+      <c r="AH7" t="n">
+        <v/>
+      </c>
+      <c r="AI7" t="n">
+        <v/>
+      </c>
+      <c r="AJ7" t="n">
+        <v/>
+      </c>
+      <c r="AK7" t="n">
+        <v/>
+      </c>
+      <c r="AL7" t="n">
+        <v/>
+      </c>
+      <c r="AM7" t="n">
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -718,6 +1052,70 @@
       <c r="N8" t="n">
         <v>243.25</v>
       </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>read</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>128k</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>703</v>
+      </c>
+      <c r="W8" t="n">
+        <v>1320</v>
+      </c>
+      <c r="X8" t="n">
+        <v>1882</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>2024</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>5626</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>177.08</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>188.33</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>196.99</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>245.16</v>
+      </c>
+      <c r="AH8" t="n">
+        <v/>
+      </c>
+      <c r="AI8" t="n">
+        <v/>
+      </c>
+      <c r="AJ8" t="n">
+        <v/>
+      </c>
+      <c r="AK8" t="n">
+        <v/>
+      </c>
+      <c r="AL8" t="n">
+        <v/>
+      </c>
+      <c r="AM8" t="n">
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
@@ -761,6 +1159,65 @@
       <c r="N9" t="n">
         <v>7853.38</v>
       </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>4k</t>
+        </is>
+      </c>
+      <c r="V9" t="n">
+        <v>865</v>
+      </c>
+      <c r="W9" t="n">
+        <v>1191</v>
+      </c>
+      <c r="X9" t="n">
+        <v>1730</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>1962</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>221000</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>305000</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>443000</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>502000</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>4408.42</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>6445.61</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>6627.87</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>7802.57</v>
+      </c>
+      <c r="AH9" t="n">
+        <v/>
+      </c>
+      <c r="AI9" t="n">
+        <v/>
+      </c>
+      <c r="AJ9" t="n">
+        <v/>
+      </c>
+      <c r="AK9" t="n">
+        <v/>
+      </c>
+      <c r="AL9" t="n">
+        <v/>
+      </c>
+      <c r="AM9" t="n">
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -809,6 +1266,70 @@
       <c r="N10" t="n">
         <v>52.51</v>
       </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>write</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>128k</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>790</v>
+      </c>
+      <c r="W10" t="n">
+        <v>892</v>
+      </c>
+      <c r="X10" t="n">
+        <v>1123</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>1662</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>6320</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>7135</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>8982</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>34161.27</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>37817.43</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>41990.04</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>47.84</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>37120</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>43776</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>47872</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>39680</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>59136</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>67072</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
@@ -852,626 +1373,63 @@
       <c r="N11" t="n">
         <v>2166.54</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>BW(MiB/s)</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>IOPS</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>lat_avg(ns)</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>lat_p95(ns)</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>lat_p99(ns)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>3</v>
-      </c>
-      <c r="J2" t="n">
-        <v>4</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2</v>
-      </c>
-      <c r="M2" t="n">
-        <v>3</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>3</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>2</v>
-      </c>
-      <c r="T2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>workload</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>bs</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>randread</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>128k</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>380</v>
-      </c>
-      <c r="D4" t="n">
-        <v>705</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1011</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1249</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3038</v>
-      </c>
-      <c r="H4" t="n">
-        <v>5641</v>
-      </c>
-      <c r="I4" t="n">
-        <v>8084</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9990</v>
-      </c>
-      <c r="K4" t="n">
-        <v>328.52</v>
-      </c>
-      <c r="L4" t="n">
-        <v>352.26</v>
-      </c>
-      <c r="M4" t="n">
-        <v>364.82</v>
-      </c>
-      <c r="N4" t="n">
-        <v>381.4</v>
-      </c>
-      <c r="O4" t="n">
-        <v/>
-      </c>
-      <c r="P4" t="n">
-        <v/>
-      </c>
-      <c r="Q4" t="n">
-        <v/>
-      </c>
-      <c r="R4" t="n">
-        <v/>
-      </c>
-      <c r="S4" t="n">
-        <v/>
-      </c>
-      <c r="T4" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>4k</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v/>
-      </c>
-      <c r="D5" t="n">
-        <v/>
-      </c>
-      <c r="E5" t="n">
-        <v/>
-      </c>
-      <c r="F5" t="n">
-        <v/>
-      </c>
-      <c r="G5" t="n">
-        <v>5818</v>
-      </c>
-      <c r="H5" t="n">
-        <v>11</v>
-      </c>
-      <c r="I5" t="n">
-        <v>16</v>
-      </c>
-      <c r="J5" t="n">
-        <v>21</v>
-      </c>
-      <c r="K5" t="n">
-        <v>5720.45</v>
-      </c>
-      <c r="L5" t="n">
-        <v>10969.64</v>
-      </c>
-      <c r="M5" t="n">
-        <v>15906</v>
-      </c>
-      <c r="N5" t="n">
-        <v>21039.03</v>
-      </c>
-      <c r="O5" t="n">
-        <v/>
-      </c>
-      <c r="P5" t="n">
-        <v/>
-      </c>
-      <c r="Q5" t="n">
-        <v/>
-      </c>
-      <c r="R5" t="n">
-        <v/>
-      </c>
-      <c r="S5" t="n">
-        <v/>
-      </c>
-      <c r="T5" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>randwrite</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>128k</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>186</v>
-      </c>
-      <c r="D6" t="n">
-        <v>197</v>
-      </c>
-      <c r="E6" t="n">
-        <v>249</v>
-      </c>
-      <c r="F6" t="n">
-        <v>290</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1484</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1572</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1989</v>
-      </c>
-      <c r="J6" t="n">
-        <v>2323</v>
-      </c>
-      <c r="K6" t="n">
-        <v>61.78</v>
-      </c>
-      <c r="L6" t="n">
-        <v>59.39</v>
-      </c>
-      <c r="M6" t="n">
-        <v>61.27</v>
-      </c>
-      <c r="N6" t="n">
-        <v>69.94</v>
-      </c>
-      <c r="O6" t="n">
-        <v/>
-      </c>
-      <c r="P6" t="n">
-        <v/>
-      </c>
-      <c r="Q6" t="n">
-        <v/>
-      </c>
-      <c r="R6" t="n">
-        <v/>
-      </c>
-      <c r="S6" t="n">
-        <v/>
-      </c>
-      <c r="T6" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>4k</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v/>
-      </c>
-      <c r="D7" t="n">
-        <v>140</v>
-      </c>
-      <c r="E7" t="n">
-        <v>150</v>
-      </c>
-      <c r="F7" t="n">
-        <v>185</v>
-      </c>
-      <c r="G7" t="n">
-        <v>17</v>
-      </c>
-      <c r="H7" t="n">
-        <v>35</v>
-      </c>
-      <c r="I7" t="n">
-        <v>38</v>
-      </c>
-      <c r="J7" t="n">
-        <v>47</v>
-      </c>
-      <c r="K7" t="n">
-        <v>30723</v>
-      </c>
-      <c r="L7" t="n">
-        <v>60528</v>
-      </c>
-      <c r="M7" t="n">
-        <v>82994</v>
-      </c>
-      <c r="N7" t="n">
-        <v>107703</v>
-      </c>
-      <c r="O7" t="n">
-        <v/>
-      </c>
-      <c r="P7" t="n">
-        <v/>
-      </c>
-      <c r="Q7" t="n">
-        <v/>
-      </c>
-      <c r="R7" t="n">
-        <v/>
-      </c>
-      <c r="S7" t="n">
-        <v/>
-      </c>
-      <c r="T7" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>read</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>128k</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>703</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1320</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1882</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2024</v>
-      </c>
-      <c r="G8" t="n">
-        <v>5626</v>
-      </c>
-      <c r="H8" t="n">
-        <v>10</v>
-      </c>
-      <c r="I8" t="n">
-        <v>15</v>
-      </c>
-      <c r="J8" t="n">
-        <v>16</v>
-      </c>
-      <c r="K8" t="n">
-        <v>177.08</v>
-      </c>
-      <c r="L8" t="n">
-        <v>188.33</v>
-      </c>
-      <c r="M8" t="n">
-        <v>196.99</v>
-      </c>
-      <c r="N8" t="n">
-        <v>245.16</v>
-      </c>
-      <c r="O8" t="n">
-        <v/>
-      </c>
-      <c r="P8" t="n">
-        <v/>
-      </c>
-      <c r="Q8" t="n">
-        <v/>
-      </c>
-      <c r="R8" t="n">
-        <v/>
-      </c>
-      <c r="S8" t="n">
-        <v/>
-      </c>
-      <c r="T8" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>4k</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>865</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1191</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1730</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1962</v>
-      </c>
-      <c r="G9" t="n">
-        <v>221000</v>
-      </c>
-      <c r="H9" t="n">
-        <v>305000</v>
-      </c>
-      <c r="I9" t="n">
-        <v>443000</v>
-      </c>
-      <c r="J9" t="n">
-        <v>502000</v>
-      </c>
-      <c r="K9" t="n">
-        <v>4408.42</v>
-      </c>
-      <c r="L9" t="n">
-        <v>6445.61</v>
-      </c>
-      <c r="M9" t="n">
-        <v>6627.87</v>
-      </c>
-      <c r="N9" t="n">
-        <v>7802.57</v>
-      </c>
-      <c r="O9" t="n">
-        <v/>
-      </c>
-      <c r="P9" t="n">
-        <v/>
-      </c>
-      <c r="Q9" t="n">
-        <v/>
-      </c>
-      <c r="R9" t="n">
-        <v/>
-      </c>
-      <c r="S9" t="n">
-        <v/>
-      </c>
-      <c r="T9" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>write</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>128k</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>790</v>
-      </c>
-      <c r="D10" t="n">
-        <v>892</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1123</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1662</v>
-      </c>
-      <c r="G10" t="n">
-        <v>6320</v>
-      </c>
-      <c r="H10" t="n">
-        <v>7135</v>
-      </c>
-      <c r="I10" t="n">
-        <v>8982</v>
-      </c>
-      <c r="J10" t="n">
-        <v>13</v>
-      </c>
-      <c r="K10" t="n">
-        <v>34161.27</v>
-      </c>
-      <c r="L10" t="n">
-        <v>37817.43</v>
-      </c>
-      <c r="M10" t="n">
-        <v>41990.04</v>
-      </c>
-      <c r="N10" t="n">
-        <v>47.84</v>
-      </c>
-      <c r="O10" t="n">
-        <v>37120</v>
-      </c>
-      <c r="P10" t="n">
-        <v>43776</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>47872</v>
-      </c>
-      <c r="R10" t="n">
-        <v>39680</v>
-      </c>
-      <c r="S10" t="n">
-        <v>59136</v>
-      </c>
-      <c r="T10" t="n">
-        <v>67072</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>4k</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+      <c r="V11" t="n">
         <v>557</v>
       </c>
-      <c r="D11" t="n">
+      <c r="W11" t="n">
         <v>1028</v>
       </c>
-      <c r="E11" t="n">
+      <c r="X11" t="n">
         <v>982</v>
       </c>
-      <c r="F11" t="n">
+      <c r="Y11" t="n">
         <v>1243</v>
       </c>
-      <c r="G11" t="n">
+      <c r="Z11" t="n">
         <v>142000</v>
       </c>
-      <c r="H11" t="n">
+      <c r="AA11" t="n">
         <v>263000</v>
       </c>
-      <c r="I11" t="n">
+      <c r="AB11" t="n">
         <v>251000</v>
       </c>
-      <c r="J11" t="n">
+      <c r="AC11" t="n">
         <v>318000</v>
       </c>
-      <c r="K11" t="n">
+      <c r="AD11" t="n">
         <v>1236.17</v>
       </c>
-      <c r="L11" t="n">
+      <c r="AE11" t="n">
         <v>1481.27</v>
       </c>
-      <c r="M11" t="n">
+      <c r="AF11" t="n">
         <v>1474.04</v>
       </c>
-      <c r="N11" t="n">
+      <c r="AG11" t="n">
         <v>1577.2</v>
       </c>
-      <c r="O11" t="n">
-        <v/>
-      </c>
-      <c r="P11" t="n">
-        <v/>
-      </c>
-      <c r="Q11" t="n">
-        <v/>
-      </c>
-      <c r="R11" t="n">
-        <v/>
-      </c>
-      <c r="S11" t="n">
-        <v/>
-      </c>
-      <c r="T11" t="n">
+      <c r="AH11" t="n">
+        <v/>
+      </c>
+      <c r="AI11" t="n">
+        <v/>
+      </c>
+      <c r="AJ11" t="n">
+        <v/>
+      </c>
+      <c r="AK11" t="n">
+        <v/>
+      </c>
+      <c r="AL11" t="n">
+        <v/>
+      </c>
+      <c r="AM11" t="n">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
noslag-gpu full eval file update
</commit_message>
<xml_diff>
--- a/rfuse/ext4_summary.xlsx
+++ b/rfuse/ext4_summary.xlsx
@@ -468,22 +468,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>8258</v>
+        <v>9394</v>
       </c>
       <c r="C3" s="3">
-        <v>15200</v>
+        <v>17400</v>
       </c>
       <c r="D3" s="3">
-        <v>27100</v>
+        <v>30100</v>
       </c>
       <c r="E3" s="3">
-        <v>37200</v>
+        <v>38500</v>
       </c>
       <c r="F3" s="3">
-        <v>38300</v>
+        <v>39100</v>
       </c>
       <c r="G3" s="3">
-        <v>38100</v>
+        <v>39500</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -491,22 +491,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>1082.130432</v>
+        <v>1231.028224</v>
       </c>
       <c r="C4" s="4">
-        <v>1988.100096</v>
+        <v>2274.361344</v>
       </c>
       <c r="D4" s="4">
-        <v>3555.721216</v>
+        <v>3947.88864</v>
       </c>
       <c r="E4" s="4">
-        <v>4881.12128</v>
+        <v>5041.553408</v>
       </c>
       <c r="F4" s="4">
-        <v>5017.43616</v>
+        <v>5125.439488</v>
       </c>
       <c r="G4" s="4">
-        <v>4988.076032</v>
+        <v>5181.014016</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -514,22 +514,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>119.76</v>
+        <v>105.5</v>
       </c>
       <c r="C5" s="4">
-        <v>130.06</v>
+        <v>113.63</v>
       </c>
       <c r="D5" s="4">
-        <v>145.82</v>
+        <v>130.56</v>
       </c>
       <c r="E5" s="4">
-        <v>211.97</v>
+        <v>205.11</v>
       </c>
       <c r="F5" s="4">
-        <v>406.72</v>
+        <v>397.32</v>
       </c>
       <c r="G5" s="4">
-        <v>818.37</v>
+        <v>788.98</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -537,22 +537,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="C6" s="4">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="D6" s="4">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="E6" s="4">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="F6" s="4">
-        <v>1106</v>
+        <v>1336</v>
       </c>
       <c r="G6" s="4">
-        <v>2802</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -560,22 +560,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="C7" s="4">
-        <v>247</v>
+        <v>204</v>
       </c>
       <c r="D7" s="4">
-        <v>289</v>
+        <v>262</v>
       </c>
       <c r="E7" s="4">
-        <v>474</v>
+        <v>502</v>
       </c>
       <c r="F7" s="4">
-        <v>1680</v>
+        <v>2024</v>
       </c>
       <c r="G7" s="4">
-        <v>4621</v>
+        <v>4359</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -617,19 +617,19 @@
         <v>35700</v>
       </c>
       <c r="C12" s="3">
-        <v>70900</v>
+        <v>71900</v>
       </c>
       <c r="D12" s="3">
-        <v>139000</v>
+        <v>142000</v>
       </c>
       <c r="E12" s="3">
-        <v>263000</v>
+        <v>271000</v>
       </c>
       <c r="F12" s="3">
-        <v>474000</v>
+        <v>482000</v>
       </c>
       <c r="G12" s="3">
-        <v>777000</v>
+        <v>774000</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -640,19 +640,19 @@
         <v>145.752064</v>
       </c>
       <c r="C13" s="4">
-        <v>290.455552</v>
+        <v>294.649856</v>
       </c>
       <c r="D13" s="4">
-        <v>570.425344</v>
+        <v>581.95968</v>
       </c>
       <c r="E13" s="4">
-        <v>1075.838976</v>
+        <v>1111.49056</v>
       </c>
       <c r="F13" s="4">
-        <v>1941.962752</v>
+        <v>1973.420032</v>
       </c>
       <c r="G13" s="4">
-        <v>3181.379584</v>
+        <v>3169.845248</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -660,22 +660,22 @@
         <v>3</v>
       </c>
       <c r="B14" s="4">
-        <v>27.65067</v>
+        <v>27.5332</v>
       </c>
       <c r="C14" s="4">
-        <v>27.78939</v>
+        <v>27.40673</v>
       </c>
       <c r="D14" s="4">
-        <v>28.27756</v>
+        <v>27.72106</v>
       </c>
       <c r="E14" s="4">
-        <v>29.57228</v>
+        <v>28.84652</v>
       </c>
       <c r="F14" s="4">
-        <v>32.73336</v>
+        <v>32.19637</v>
       </c>
       <c r="G14" s="4">
-        <v>39.99583000000001</v>
+        <v>40.59279</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -686,19 +686,19 @@
         <v>44.288</v>
       </c>
       <c r="C15" s="4">
-        <v>44.8</v>
+        <v>44.288</v>
       </c>
       <c r="D15" s="4">
-        <v>46.336</v>
+        <v>45.312</v>
       </c>
       <c r="E15" s="4">
-        <v>50.432</v>
+        <v>48.896</v>
       </c>
       <c r="F15" s="4">
-        <v>60.672</v>
+        <v>59.648</v>
       </c>
       <c r="G15" s="4">
-        <v>81.408</v>
+        <v>82.432</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -706,22 +706,22 @@
         <v>5</v>
       </c>
       <c r="B16" s="4">
+        <v>45.824</v>
+      </c>
+      <c r="C16" s="4">
         <v>46.848</v>
       </c>
-      <c r="C16" s="4">
-        <v>48.384</v>
-      </c>
       <c r="D16" s="4">
-        <v>54.528</v>
+        <v>53.504</v>
       </c>
       <c r="E16" s="4">
-        <v>64.256</v>
+        <v>63.232</v>
       </c>
       <c r="F16" s="4">
         <v>75.264</v>
       </c>
       <c r="G16" s="4">
-        <v>101.888</v>
+        <v>102.912</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -760,22 +760,22 @@
         <v>1</v>
       </c>
       <c r="B21" s="3">
-        <v>8982</v>
+        <v>12000</v>
       </c>
       <c r="C21" s="3">
-        <v>13200</v>
+        <v>18100</v>
       </c>
       <c r="D21" s="3">
-        <v>17900</v>
+        <v>22800</v>
       </c>
       <c r="E21" s="3">
-        <v>19000</v>
+        <v>26900</v>
       </c>
       <c r="F21" s="3">
-        <v>22700</v>
+        <v>29300</v>
       </c>
       <c r="G21" s="3">
-        <v>21700</v>
+        <v>24200</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -783,22 +783,22 @@
         <v>2</v>
       </c>
       <c r="B22" s="4">
-        <v>1177.550848</v>
+        <v>1579.155456</v>
       </c>
       <c r="C22" s="4">
-        <v>1732.247552</v>
+        <v>2375.02464</v>
       </c>
       <c r="D22" s="4">
-        <v>2344.615936</v>
+        <v>2982.150144</v>
       </c>
       <c r="E22" s="4">
-        <v>2619.342848</v>
+        <v>3520.069632</v>
       </c>
       <c r="F22" s="4">
-        <v>2977.95584</v>
+        <v>3834.642432</v>
       </c>
       <c r="G22" s="4">
-        <v>2838.495232</v>
+        <v>3177.18528</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -806,22 +806,22 @@
         <v>3</v>
       </c>
       <c r="B23" s="4">
-        <v>78.14</v>
+        <v>49.98</v>
       </c>
       <c r="C23" s="4">
-        <v>86.52</v>
+        <v>51.12</v>
       </c>
       <c r="D23" s="4">
-        <v>105.28</v>
+        <v>55.24</v>
       </c>
       <c r="E23" s="4">
-        <v>196.39</v>
+        <v>79.20999999999999</v>
       </c>
       <c r="F23" s="4">
-        <v>385.97</v>
+        <v>190.42</v>
       </c>
       <c r="G23" s="4">
-        <v>661.5599999999999</v>
+        <v>574.36</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -829,22 +829,22 @@
         <v>4</v>
       </c>
       <c r="B24" s="4">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C24" s="4">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="D24" s="4">
-        <v>151</v>
+        <v>72</v>
       </c>
       <c r="E24" s="4">
-        <v>260</v>
+        <v>106</v>
       </c>
       <c r="F24" s="4">
-        <v>676</v>
+        <v>310</v>
       </c>
       <c r="G24" s="4">
-        <v>1303</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -852,19 +852,19 @@
         <v>5</v>
       </c>
       <c r="B25" s="4">
-        <v>396</v>
+        <v>155</v>
       </c>
       <c r="C25" s="4">
-        <v>188</v>
+        <v>85</v>
       </c>
       <c r="D25" s="4">
-        <v>186</v>
+        <v>103</v>
       </c>
       <c r="E25" s="4">
-        <v>289</v>
+        <v>123</v>
       </c>
       <c r="F25" s="4">
-        <v>775</v>
+        <v>392</v>
       </c>
       <c r="G25" s="4">
         <v>2540</v>
@@ -906,22 +906,22 @@
         <v>1</v>
       </c>
       <c r="B30" s="3">
-        <v>185000</v>
+        <v>239000</v>
       </c>
       <c r="C30" s="3">
-        <v>333000</v>
+        <v>423000</v>
       </c>
       <c r="D30" s="3">
-        <v>514000</v>
+        <v>630000</v>
       </c>
       <c r="E30" s="3">
-        <v>597000</v>
+        <v>771000</v>
       </c>
       <c r="F30" s="3">
-        <v>667000</v>
+        <v>685000</v>
       </c>
       <c r="G30" s="3">
-        <v>370000</v>
+        <v>680000</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -929,22 +929,22 @@
         <v>2</v>
       </c>
       <c r="B31" s="4">
-        <v>758.120448</v>
+        <v>979.369984</v>
       </c>
       <c r="C31" s="4">
-        <v>1362.100224</v>
+        <v>1732.247552</v>
       </c>
       <c r="D31" s="4">
-        <v>2105.540608</v>
+        <v>2581.594112</v>
       </c>
       <c r="E31" s="4">
-        <v>2446.327808</v>
+        <v>3158.310912</v>
       </c>
       <c r="F31" s="4">
-        <v>2732.589056</v>
+        <v>2807.037952</v>
       </c>
       <c r="G31" s="4">
-        <v>1515.19232</v>
+        <v>2785.017856</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -952,22 +952,22 @@
         <v>3</v>
       </c>
       <c r="B32" s="4">
-        <v>3.29691</v>
+        <v>2.22498</v>
       </c>
       <c r="C32" s="4">
-        <v>3.53023</v>
+        <v>2.38901</v>
       </c>
       <c r="D32" s="4">
-        <v>3.79462</v>
+        <v>2.39453</v>
       </c>
       <c r="E32" s="4">
-        <v>6.018470000000001</v>
+        <v>2.61313</v>
       </c>
       <c r="F32" s="4">
-        <v>11.45276</v>
+        <v>4.92057</v>
       </c>
       <c r="G32" s="4">
-        <v>20.06463</v>
+        <v>16.83237</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -975,22 +975,22 @@
         <v>4</v>
       </c>
       <c r="B33" s="4">
-        <v>6.88</v>
+        <v>3.568</v>
       </c>
       <c r="C33" s="4">
-        <v>7.136</v>
+        <v>3.952</v>
       </c>
       <c r="D33" s="4">
-        <v>7.072</v>
+        <v>3.952</v>
       </c>
       <c r="E33" s="4">
-        <v>9.024000000000001</v>
+        <v>4.256</v>
       </c>
       <c r="F33" s="4">
-        <v>21.888</v>
+        <v>9.536</v>
       </c>
       <c r="G33" s="4">
-        <v>42.24</v>
+        <v>55.552</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -998,22 +998,22 @@
         <v>5</v>
       </c>
       <c r="B34" s="4">
-        <v>8.096</v>
+        <v>4.832</v>
       </c>
       <c r="C34" s="4">
-        <v>8.640000000000001</v>
+        <v>5.28</v>
       </c>
       <c r="D34" s="4">
-        <v>8.768000000000001</v>
+        <v>5.344</v>
       </c>
       <c r="E34" s="4">
-        <v>12.608</v>
+        <v>5.92</v>
       </c>
       <c r="F34" s="4">
-        <v>29.568</v>
+        <v>13.248</v>
       </c>
       <c r="G34" s="4">
-        <v>79.36</v>
+        <v>84.48</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1052,22 +1052,22 @@
         <v>1</v>
       </c>
       <c r="B39" s="3">
-        <v>12300</v>
+        <v>18300</v>
       </c>
       <c r="C39" s="3">
-        <v>21600</v>
+        <v>24700</v>
       </c>
       <c r="D39" s="3">
-        <v>23000</v>
+        <v>24400</v>
       </c>
       <c r="E39" s="3">
-        <v>24200</v>
+        <v>24700</v>
       </c>
       <c r="F39" s="3">
-        <v>24500</v>
+        <v>25000</v>
       </c>
       <c r="G39" s="3">
-        <v>24600</v>
+        <v>25100</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1075,22 +1075,22 @@
         <v>2</v>
       </c>
       <c r="B40" s="4">
-        <v>1616.904192</v>
+        <v>2397.044736</v>
       </c>
       <c r="C40" s="4">
-        <v>2825.91232</v>
+        <v>3233.808384</v>
       </c>
       <c r="D40" s="4">
-        <v>3139.436544</v>
+        <v>3196.059648</v>
       </c>
       <c r="E40" s="4">
-        <v>3167.748096</v>
+        <v>3244.294144</v>
       </c>
       <c r="F40" s="4">
-        <v>3214.934016</v>
+        <v>3278.897152</v>
       </c>
       <c r="G40" s="4">
-        <v>3229.61408</v>
+        <v>3291.480064</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1098,22 +1098,22 @@
         <v>3</v>
       </c>
       <c r="B41" s="4">
-        <v>79.83</v>
+        <v>54.35</v>
       </c>
       <c r="C41" s="4">
-        <v>89.47</v>
+        <v>79.76000000000001</v>
       </c>
       <c r="D41" s="4">
-        <v>163.3</v>
+        <v>162.17</v>
       </c>
       <c r="E41" s="4">
-        <v>325.81</v>
+        <v>320.93</v>
       </c>
       <c r="F41" s="4">
-        <v>645.28</v>
+        <v>637.24</v>
       </c>
       <c r="G41" s="4">
-        <v>1287.33</v>
+        <v>1270.21</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1121,22 +1121,22 @@
         <v>4</v>
       </c>
       <c r="B42" s="4">
-        <v>157</v>
+        <v>92</v>
       </c>
       <c r="C42" s="4">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="D42" s="4">
-        <v>562</v>
+        <v>586</v>
       </c>
       <c r="E42" s="4">
-        <v>1336</v>
+        <v>1516</v>
       </c>
       <c r="F42" s="4">
-        <v>3228</v>
+        <v>3752</v>
       </c>
       <c r="G42" s="4">
-        <v>6980</v>
+        <v>7046</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1144,19 +1144,19 @@
         <v>5</v>
       </c>
       <c r="B43" s="4">
-        <v>225</v>
+        <v>95</v>
       </c>
       <c r="C43" s="4">
-        <v>241</v>
+        <v>145</v>
       </c>
       <c r="D43" s="4">
-        <v>791</v>
+        <v>775</v>
       </c>
       <c r="E43" s="4">
-        <v>1844</v>
+        <v>2073</v>
       </c>
       <c r="F43" s="4">
-        <v>4293</v>
+        <v>4555</v>
       </c>
       <c r="G43" s="4">
         <v>7898</v>
@@ -1198,22 +1198,22 @@
         <v>1</v>
       </c>
       <c r="B48" s="3">
-        <v>368000</v>
+        <v>462000</v>
       </c>
       <c r="C48" s="3">
-        <v>618000</v>
+        <v>790000</v>
       </c>
       <c r="D48" s="3">
-        <v>753000</v>
+        <v>776000</v>
       </c>
       <c r="E48" s="3">
-        <v>771000</v>
+        <v>797000</v>
       </c>
       <c r="F48" s="3">
-        <v>783000</v>
+        <v>802000</v>
       </c>
       <c r="G48" s="3">
-        <v>759000</v>
+        <v>804000</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1221,22 +1221,22 @@
         <v>2</v>
       </c>
       <c r="B49" s="4">
-        <v>1507.852288</v>
+        <v>1890.582528</v>
       </c>
       <c r="C49" s="4">
-        <v>2532.31104</v>
+        <v>3233.808384</v>
       </c>
       <c r="D49" s="4">
-        <v>3085.959168</v>
+        <v>3177.18528</v>
       </c>
       <c r="E49" s="4">
-        <v>3158.310912</v>
+        <v>3263.168512</v>
       </c>
       <c r="F49" s="4">
-        <v>3205.496832</v>
+        <v>3283.091456</v>
       </c>
       <c r="G49" s="4">
-        <v>3110.076416</v>
+        <v>3291.480064</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1244,22 +1244,22 @@
         <v>3</v>
       </c>
       <c r="B50" s="4">
-        <v>2.4471</v>
+        <v>1.94216</v>
       </c>
       <c r="C50" s="4">
-        <v>2.96363</v>
+        <v>2.2863</v>
       </c>
       <c r="D50" s="4">
-        <v>5.00722</v>
+        <v>4.852270000000001</v>
       </c>
       <c r="E50" s="4">
-        <v>10.03239</v>
+        <v>9.763030000000001</v>
       </c>
       <c r="F50" s="4">
-        <v>19.80364</v>
+        <v>19.67969</v>
       </c>
       <c r="G50" s="4">
-        <v>41.54157</v>
+        <v>39.52358</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1267,22 +1267,22 @@
         <v>4</v>
       </c>
       <c r="B51" s="4">
-        <v>1.304</v>
+        <v>0.908</v>
       </c>
       <c r="C51" s="4">
-        <v>1.4</v>
+        <v>0.972</v>
       </c>
       <c r="D51" s="4">
-        <v>1.512</v>
+        <v>1.064</v>
       </c>
       <c r="E51" s="4">
-        <v>2.096</v>
+        <v>1.192</v>
       </c>
       <c r="F51" s="4">
-        <v>6.56</v>
+        <v>1.256</v>
       </c>
       <c r="G51" s="4">
-        <v>7.264</v>
+        <v>1.368</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1290,22 +1290,22 @@
         <v>5</v>
       </c>
       <c r="B52" s="4">
-        <v>111.104</v>
+        <v>74.23999999999999</v>
       </c>
       <c r="C52" s="4">
-        <v>134.144</v>
+        <v>93.696</v>
       </c>
       <c r="D52" s="4">
-        <v>171.008</v>
+        <v>138.24</v>
       </c>
       <c r="E52" s="4">
-        <v>350.208</v>
+        <v>257.024</v>
       </c>
       <c r="F52" s="4">
-        <v>536.576</v>
+        <v>284.672</v>
       </c>
       <c r="G52" s="4">
-        <v>749.568</v>
+        <v>284.672</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1344,22 +1344,22 @@
         <v>1</v>
       </c>
       <c r="B57" s="3">
-        <v>7211</v>
+        <v>9570</v>
       </c>
       <c r="C57" s="3">
-        <v>10800</v>
+        <v>13500</v>
       </c>
       <c r="D57" s="3">
-        <v>13700</v>
+        <v>17100</v>
       </c>
       <c r="E57" s="3">
-        <v>14900</v>
+        <v>16000</v>
       </c>
       <c r="F57" s="3">
-        <v>16000</v>
+        <v>16800</v>
       </c>
       <c r="G57" s="3">
-        <v>17800</v>
+        <v>18900</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1367,22 +1367,22 @@
         <v>2</v>
       </c>
       <c r="B58" s="4">
-        <v>944.766976</v>
+        <v>1254.096896</v>
       </c>
       <c r="C58" s="4">
-        <v>1412.431872</v>
+        <v>1765.801984</v>
       </c>
       <c r="D58" s="4">
-        <v>1789.919232</v>
+        <v>2236.612608</v>
       </c>
       <c r="E58" s="4">
-        <v>1955.59424</v>
+        <v>2222.98112</v>
       </c>
       <c r="F58" s="4">
-        <v>2097.152</v>
+        <v>2203.058176</v>
       </c>
       <c r="G58" s="4">
-        <v>2329.935872</v>
+        <v>2478.833664</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1390,22 +1390,22 @@
         <v>3</v>
       </c>
       <c r="B59" s="4">
-        <v>87.56</v>
+        <v>53.12981</v>
       </c>
       <c r="C59" s="4">
-        <v>93.48999999999999</v>
+        <v>55.11626</v>
       </c>
       <c r="D59" s="4">
-        <v>110.73</v>
+        <v>56.1767</v>
       </c>
       <c r="E59" s="4">
-        <v>199.21</v>
+        <v>76.48999999999999</v>
       </c>
       <c r="F59" s="4">
-        <v>395.43</v>
+        <v>420.63</v>
       </c>
       <c r="G59" s="4">
-        <v>909.34</v>
+        <v>836.58</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1413,22 +1413,22 @@
         <v>4</v>
       </c>
       <c r="B60" s="4">
-        <v>143</v>
+        <v>56.064</v>
       </c>
       <c r="C60" s="4">
-        <v>143</v>
+        <v>58.112</v>
       </c>
       <c r="D60" s="4">
-        <v>155</v>
+        <v>59.648</v>
       </c>
       <c r="E60" s="4">
-        <v>227</v>
+        <v>88</v>
       </c>
       <c r="F60" s="4">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="G60" s="4">
-        <v>947</v>
+        <v>898</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1436,22 +1436,22 @@
         <v>5</v>
       </c>
       <c r="B61" s="4">
-        <v>149</v>
+        <v>58.112</v>
       </c>
       <c r="C61" s="4">
-        <v>151</v>
+        <v>62.208</v>
       </c>
       <c r="D61" s="4">
-        <v>167</v>
+        <v>63.232</v>
       </c>
       <c r="E61" s="4">
-        <v>247</v>
+        <v>96</v>
       </c>
       <c r="F61" s="4">
         <v>578</v>
       </c>
       <c r="G61" s="4">
-        <v>17171</v>
+        <v>21365</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1490,19 +1490,19 @@
         <v>1</v>
       </c>
       <c r="B66" s="3">
-        <v>204000</v>
+        <v>264000</v>
       </c>
       <c r="C66" s="3">
-        <v>315000</v>
+        <v>388000</v>
       </c>
       <c r="D66" s="3">
-        <v>434000</v>
+        <v>506000</v>
       </c>
       <c r="E66" s="3">
-        <v>466000</v>
+        <v>542000</v>
       </c>
       <c r="F66" s="3">
-        <v>512000</v>
+        <v>605000</v>
       </c>
       <c r="G66" s="3">
         <v>563000</v>
@@ -1513,43 +1513,45 @@
         <v>2</v>
       </c>
       <c r="B67" s="4">
-        <v>833.61792</v>
+        <v>1082.130432</v>
       </c>
       <c r="C67" s="4">
-        <v>1290.797056</v>
+        <v>1588.59264</v>
       </c>
       <c r="D67" s="4">
-        <v>1777.33632</v>
+        <v>2073.034752</v>
       </c>
       <c r="E67" s="4">
-        <v>1907.359744</v>
+        <v>2218.786816</v>
       </c>
       <c r="F67" s="4">
-        <v>2097.152</v>
+        <v>2476.736512</v>
       </c>
       <c r="G67" s="4">
-        <v>2303.721472</v>
+        <v>2305.818624</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="4"/>
+      <c r="B68" s="4">
+        <v>2.01044</v>
+      </c>
       <c r="C68" s="4">
-        <v>3.22242</v>
+        <v>2.08489</v>
       </c>
       <c r="D68" s="4">
-        <v>3.57382</v>
+        <v>2.12109</v>
       </c>
       <c r="E68" s="4">
-        <v>6.077560000000001</v>
+        <v>2.34079</v>
       </c>
       <c r="F68" s="4">
-        <v>14.2809</v>
+        <v>4.81608</v>
       </c>
       <c r="G68" s="4">
-        <v>27.89419</v>
+        <v>30.10735</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1557,22 +1559,22 @@
         <v>4</v>
       </c>
       <c r="B69" s="4">
-        <v>5.344</v>
+        <v>2.896</v>
       </c>
       <c r="C69" s="4">
-        <v>5.536</v>
+        <v>3.216</v>
       </c>
       <c r="D69" s="4">
-        <v>5.792</v>
+        <v>3.344</v>
       </c>
       <c r="E69" s="4">
-        <v>8.768000000000001</v>
+        <v>3.792</v>
       </c>
       <c r="F69" s="4">
-        <v>19.584</v>
+        <v>8.512</v>
       </c>
       <c r="G69" s="4">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -1580,22 +1582,22 @@
         <v>5</v>
       </c>
       <c r="B70" s="4">
-        <v>7.008</v>
+        <v>4.192</v>
       </c>
       <c r="C70" s="4">
-        <v>7.136</v>
+        <v>4.64</v>
       </c>
       <c r="D70" s="4">
-        <v>8.256</v>
+        <v>4.576000000000001</v>
       </c>
       <c r="E70" s="4">
-        <v>12.48</v>
+        <v>5.792</v>
       </c>
       <c r="F70" s="4">
-        <v>27.264</v>
+        <v>11.968</v>
       </c>
       <c r="G70" s="4">
-        <v>161</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>